<commit_message>
improved apperance and fixed litle bugs
</commit_message>
<xml_diff>
--- a/population.xlsx
+++ b/population.xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">powiat bydgoski</t>
   </si>
   <si>
-    <t xml:space="preserve">powiat Bydgoszcz</t>
+    <t xml:space="preserve">Bydgoszcz</t>
   </si>
   <si>
     <t xml:space="preserve">Bytom</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">powiat bytowski</t>
   </si>
   <si>
-    <t xml:space="preserve">powiat  Chełm</t>
+    <t xml:space="preserve">Chełm</t>
   </si>
   <si>
     <t xml:space="preserve">powiat chełmiński</t>
@@ -1287,10 +1287,10 @@
   <dimension ref="A1:E381"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.21"/>
   </cols>
@@ -6262,7 +6262,7 @@
     <hyperlink ref="A9" r:id="rId10" display="powiat białobrzeski"/>
     <hyperlink ref="A10" r:id="rId11" display="powiat białogardzki"/>
     <hyperlink ref="A11" r:id="rId12" display="powiat białostocki"/>
-    <hyperlink ref="A12" r:id="rId13" display="Białystok"/>
+    <hyperlink ref="A12" r:id="rId13" display="powiat Białystok"/>
     <hyperlink ref="A13" r:id="rId14" display="powiat bielski"/>
     <hyperlink ref="A14" r:id="rId15" display="powiat bielski"/>
     <hyperlink ref="A15" r:id="rId16" display="Bielsko-Biała"/>
@@ -6279,359 +6279,357 @@
     <hyperlink ref="A26" r:id="rId27" display="powiat brzozowski"/>
     <hyperlink ref="A27" r:id="rId28" display="powiat buski"/>
     <hyperlink ref="A28" r:id="rId29" display="powiat bydgoski"/>
-    <hyperlink ref="A29" r:id="rId30" display="Bydgoszcz"/>
-    <hyperlink ref="A30" r:id="rId31" display="Bytom"/>
-    <hyperlink ref="A31" r:id="rId32" display="powiat bytowski"/>
-    <hyperlink ref="A32" r:id="rId33" display="Chełm"/>
-    <hyperlink ref="A33" r:id="rId34" display="powiat chełmiński"/>
-    <hyperlink ref="A34" r:id="rId35" display="powiat chełmski"/>
-    <hyperlink ref="A35" r:id="rId36" display="powiat chodzieski"/>
-    <hyperlink ref="A36" r:id="rId37" display="powiat chojnicki"/>
-    <hyperlink ref="A37" r:id="rId38" display="Chorzów"/>
-    <hyperlink ref="A38" r:id="rId39" display="powiat choszczeński"/>
-    <hyperlink ref="A39" r:id="rId40" display="powiat chrzanowski"/>
-    <hyperlink ref="A40" r:id="rId41" display="powiat ciechanowski"/>
-    <hyperlink ref="A41" r:id="rId42" display="powiat cieszyński"/>
-    <hyperlink ref="A42" r:id="rId43" display="powiat czarnkowsko-trzcianecki"/>
-    <hyperlink ref="A43" r:id="rId44" display="Częstochowa"/>
-    <hyperlink ref="A44" r:id="rId45" display="powiat częstochowski"/>
-    <hyperlink ref="A45" r:id="rId46" display="powiat człuchowski"/>
-    <hyperlink ref="A46" r:id="rId47" display="Dąbrowa Górnicza"/>
-    <hyperlink ref="A47" r:id="rId48" display="powiat dąbrowski"/>
-    <hyperlink ref="A48" r:id="rId49" display="powiat dębicki"/>
-    <hyperlink ref="A49" r:id="rId50" display="powiat drawski"/>
-    <hyperlink ref="A50" r:id="rId51" display="powiat działdowski"/>
-    <hyperlink ref="A51" r:id="rId52" display="powiat dzierżoniowski"/>
-    <hyperlink ref="A52" r:id="rId53" display="Elbląg"/>
-    <hyperlink ref="A53" r:id="rId54" display="powiat elbląski"/>
-    <hyperlink ref="A54" r:id="rId55" display="powiat ełcki"/>
-    <hyperlink ref="A55" r:id="rId56" display="powiat garwoliński"/>
-    <hyperlink ref="A56" r:id="rId57" display="Gdańsk"/>
-    <hyperlink ref="A57" r:id="rId58" display="powiat gdański"/>
-    <hyperlink ref="A58" r:id="rId59" display="Gdynia"/>
-    <hyperlink ref="A59" r:id="rId60" display="powiat giżycki"/>
-    <hyperlink ref="A60" r:id="rId61" display="Gliwice"/>
-    <hyperlink ref="A61" r:id="rId62" display="powiat gliwicki"/>
-    <hyperlink ref="A62" r:id="rId63" display="powiat głogowski"/>
-    <hyperlink ref="A63" r:id="rId64" display="powiat głubczycki"/>
-    <hyperlink ref="A64" r:id="rId65" display="powiat gnieźnieński"/>
-    <hyperlink ref="A65" r:id="rId66" display="powiat goleniowski"/>
-    <hyperlink ref="A66" r:id="rId67" display="powiat golubsko-dobrzyński"/>
-    <hyperlink ref="A67" r:id="rId68" display="powiat gołdapski"/>
-    <hyperlink ref="A68" r:id="rId69" display="powiat gorlicki"/>
-    <hyperlink ref="A69" r:id="rId70" display="powiat gorzowski"/>
-    <hyperlink ref="A70" r:id="rId71" display="Gorzów Wielkopolski"/>
-    <hyperlink ref="A71" r:id="rId72" display="powiat gostyniński"/>
-    <hyperlink ref="A72" r:id="rId73" display="powiat gostyński"/>
-    <hyperlink ref="A73" r:id="rId74" display="powiat górowski"/>
-    <hyperlink ref="A74" r:id="rId75" display="powiat grajewski"/>
-    <hyperlink ref="A75" r:id="rId76" display="powiat grodziski"/>
-    <hyperlink ref="A76" r:id="rId77" display="powiat grodziski"/>
-    <hyperlink ref="A77" r:id="rId78" display="powiat grójecki"/>
-    <hyperlink ref="A78" r:id="rId79" display="Grudziądz"/>
-    <hyperlink ref="A79" r:id="rId80" display="powiat grudziądzki"/>
-    <hyperlink ref="A80" r:id="rId81" display="powiat gryficki"/>
-    <hyperlink ref="A81" r:id="rId82" display="powiat gryfiński"/>
-    <hyperlink ref="A82" r:id="rId83" display="powiat hajnowski"/>
-    <hyperlink ref="A83" r:id="rId84" display="powiat hrubieszowski"/>
-    <hyperlink ref="A84" r:id="rId85" display="powiat iławski"/>
-    <hyperlink ref="A85" r:id="rId86" display="powiat inowrocławski"/>
-    <hyperlink ref="A86" r:id="rId87" display="powiat janowski"/>
-    <hyperlink ref="A87" r:id="rId88" display="powiat jarociński"/>
-    <hyperlink ref="A88" r:id="rId89" display="powiat jarosławski"/>
-    <hyperlink ref="A89" r:id="rId90" display="powiat jasielski"/>
-    <hyperlink ref="A90" r:id="rId91" display="Jastrzębie-Zdrój"/>
-    <hyperlink ref="A91" r:id="rId92" display="powiat jaworski"/>
-    <hyperlink ref="A92" r:id="rId93" display="Jaworzno"/>
-    <hyperlink ref="A93" r:id="rId94" display="Jelenia Góra"/>
-    <hyperlink ref="A94" r:id="rId95" display="powiat jeleniogórski"/>
-    <hyperlink ref="A95" r:id="rId96" display="powiat jędrzejowski"/>
-    <hyperlink ref="A96" r:id="rId97" display="powiat kaliski"/>
-    <hyperlink ref="A97" r:id="rId98" display="Kalisz"/>
-    <hyperlink ref="A98" r:id="rId99" display="powiat kamiennogórski"/>
-    <hyperlink ref="A99" r:id="rId100" display="powiat kamieński"/>
-    <hyperlink ref="A100" r:id="rId101" display="powiat kartuski"/>
-    <hyperlink ref="A101" r:id="rId102" display="Katowice"/>
-    <hyperlink ref="A102" r:id="rId103" display="powiat kazimierski"/>
-    <hyperlink ref="A103" r:id="rId104" display="powiat kędzierzyńsko-kozielski"/>
-    <hyperlink ref="A104" r:id="rId105" display="powiat kępiński"/>
-    <hyperlink ref="A105" r:id="rId106" display="powiat kętrzyński"/>
-    <hyperlink ref="A106" r:id="rId107" display="Kielce"/>
-    <hyperlink ref="A107" r:id="rId108" display="powiat kielecki"/>
-    <hyperlink ref="A108" r:id="rId109" display="powiat kluczborski"/>
-    <hyperlink ref="A109" r:id="rId110" display="powiat kłobucki"/>
-    <hyperlink ref="A110" r:id="rId111" display="powiat kłodzki"/>
-    <hyperlink ref="A111" r:id="rId112" display="powiat kolbuszowski"/>
-    <hyperlink ref="A112" r:id="rId113" display="powiat kolneński"/>
-    <hyperlink ref="A113" r:id="rId114" display="powiat kolski"/>
-    <hyperlink ref="A114" r:id="rId115" display="powiat kołobrzeski"/>
-    <hyperlink ref="A115" r:id="rId116" display="powiat konecki"/>
-    <hyperlink ref="A116" r:id="rId117" display="Konin"/>
-    <hyperlink ref="A117" r:id="rId118" display="powiat koniński"/>
-    <hyperlink ref="A118" r:id="rId119" display="Koszalin"/>
-    <hyperlink ref="A119" r:id="rId120" display="powiat koszaliński"/>
-    <hyperlink ref="A120" r:id="rId121" display="powiat kościański"/>
-    <hyperlink ref="A121" r:id="rId122" display="powiat kościerski"/>
-    <hyperlink ref="A122" r:id="rId123" display="powiat kozienicki"/>
-    <hyperlink ref="A123" r:id="rId124" display="powiat krakowski"/>
-    <hyperlink ref="A124" r:id="rId125" display="Kraków"/>
-    <hyperlink ref="A125" r:id="rId126" display="powiat krapkowicki"/>
-    <hyperlink ref="A126" r:id="rId127" display="powiat krasnostawski"/>
-    <hyperlink ref="A127" r:id="rId128" display="powiat kraśnicki"/>
-    <hyperlink ref="A128" r:id="rId129" display="Krosno"/>
-    <hyperlink ref="A129" r:id="rId130" display="powiat krośnieński"/>
-    <hyperlink ref="A130" r:id="rId131" display="powiat krośnieński"/>
-    <hyperlink ref="A131" r:id="rId132" display="powiat krotoszyński"/>
-    <hyperlink ref="A132" r:id="rId133" display="powiat kutnowski"/>
-    <hyperlink ref="A133" r:id="rId134" display="powiat kwidzyński"/>
-    <hyperlink ref="A134" r:id="rId135" display="powiat legionowski"/>
-    <hyperlink ref="A135" r:id="rId136" display="Legnica"/>
-    <hyperlink ref="A136" r:id="rId137" display="powiat legnicki"/>
-    <hyperlink ref="A137" r:id="rId138" display="powiat leski"/>
-    <hyperlink ref="A138" r:id="rId139" display="powiat leszczyński"/>
-    <hyperlink ref="A139" r:id="rId140" display="Leszno"/>
-    <hyperlink ref="A140" r:id="rId141" display="powiat leżajski"/>
-    <hyperlink ref="A141" r:id="rId142" display="powiat lęborski"/>
-    <hyperlink ref="A142" r:id="rId143" display="powiat lidzbarski"/>
-    <hyperlink ref="A143" r:id="rId144" display="powiat limanowski"/>
-    <hyperlink ref="A144" r:id="rId145" display="powiat lipnowski"/>
-    <hyperlink ref="A145" r:id="rId146" display="powiat lipski"/>
-    <hyperlink ref="A146" r:id="rId147" display="powiat lubaczowski"/>
-    <hyperlink ref="A147" r:id="rId148" display="powiat lubański"/>
-    <hyperlink ref="A148" r:id="rId149" display="powiat lubartowski"/>
-    <hyperlink ref="A149" r:id="rId150" display="powiat lubelski"/>
-    <hyperlink ref="A150" r:id="rId151" display="powiat lubiński"/>
-    <hyperlink ref="A151" r:id="rId152" display="Lublin"/>
-    <hyperlink ref="A152" r:id="rId153" display="powiat lubliniecki"/>
-    <hyperlink ref="A153" r:id="rId154" display="powiat lwówecki"/>
-    <hyperlink ref="A154" r:id="rId155" display="powiat łańcucki"/>
-    <hyperlink ref="A155" r:id="rId156" display="powiat łaski"/>
-    <hyperlink ref="A156" r:id="rId157" display="powiat łęczycki"/>
-    <hyperlink ref="A157" r:id="rId158" display="powiat łęczyński"/>
-    <hyperlink ref="A158" r:id="rId159" display="powiat łobeski"/>
-    <hyperlink ref="A159" r:id="rId160" display="Łomża"/>
-    <hyperlink ref="A160" r:id="rId161" display="powiat łomżyński"/>
-    <hyperlink ref="A161" r:id="rId162" display="powiat łosicki"/>
-    <hyperlink ref="A162" r:id="rId163" display="powiat łowicki"/>
-    <hyperlink ref="A163" r:id="rId164" display="powiat łódzki wschodni"/>
-    <hyperlink ref="A164" r:id="rId165" display="Łódź"/>
-    <hyperlink ref="A165" r:id="rId166" display="powiat łukowski"/>
-    <hyperlink ref="A166" r:id="rId167" display="powiat makowski"/>
-    <hyperlink ref="A167" r:id="rId168" display="powiat malborski"/>
-    <hyperlink ref="A168" r:id="rId169" display="powiat miechowski"/>
-    <hyperlink ref="A169" r:id="rId170" display="powiat mielecki"/>
-    <hyperlink ref="A170" r:id="rId171" display="powiat międzychodzki"/>
-    <hyperlink ref="A171" r:id="rId172" display="powiat międzyrzecki"/>
-    <hyperlink ref="A172" r:id="rId173" display="powiat mikołowski"/>
-    <hyperlink ref="A173" r:id="rId174" display="powiat milicki"/>
-    <hyperlink ref="A174" r:id="rId175" display="powiat miński"/>
-    <hyperlink ref="A175" r:id="rId176" display="powiat mławski"/>
-    <hyperlink ref="A176" r:id="rId177" display="powiat mogileński"/>
-    <hyperlink ref="A177" r:id="rId178" display="powiat moniecki"/>
-    <hyperlink ref="A178" r:id="rId179" display="powiat mrągowski"/>
-    <hyperlink ref="A179" r:id="rId180" display="Mysłowice"/>
-    <hyperlink ref="A180" r:id="rId181" display="powiat myszkowski"/>
-    <hyperlink ref="A181" r:id="rId182" display="powiat myślenicki"/>
-    <hyperlink ref="A182" r:id="rId183" display="powiat myśliborski"/>
-    <hyperlink ref="A183" r:id="rId184" display="powiat nakielski"/>
-    <hyperlink ref="A184" r:id="rId185" display="powiat namysłowski"/>
-    <hyperlink ref="A185" r:id="rId186" display="powiat nidzicki"/>
-    <hyperlink ref="A186" r:id="rId187" display="powiat niżański"/>
-    <hyperlink ref="A187" r:id="rId188" display="powiat nowodworski"/>
-    <hyperlink ref="A188" r:id="rId189" display="powiat nowodworski"/>
-    <hyperlink ref="A189" r:id="rId190" display="powiat nowomiejski"/>
-    <hyperlink ref="A190" r:id="rId191" display="powiat nowosądecki"/>
-    <hyperlink ref="A191" r:id="rId192" display="powiat nowosolski"/>
-    <hyperlink ref="A192" r:id="rId193" display="powiat nowotarski"/>
-    <hyperlink ref="A193" r:id="rId194" display="powiat nowotomyski"/>
-    <hyperlink ref="A194" r:id="rId195" display="Nowy Sącz"/>
-    <hyperlink ref="A195" r:id="rId196" display="powiat nyski"/>
-    <hyperlink ref="A196" r:id="rId197" display="powiat obornicki"/>
-    <hyperlink ref="A197" r:id="rId198" display="powiat olecki"/>
-    <hyperlink ref="A198" r:id="rId199" display="powiat oleski"/>
-    <hyperlink ref="A199" r:id="rId200" display="powiat oleśnicki"/>
-    <hyperlink ref="A200" r:id="rId201" display="powiat olkuski"/>
-    <hyperlink ref="A201" r:id="rId202" display="Olsztyn"/>
-    <hyperlink ref="A202" r:id="rId203" display="powiat olsztyński"/>
-    <hyperlink ref="A203" r:id="rId204" display="powiat oławski"/>
-    <hyperlink ref="A204" r:id="rId205" display="powiat opatowski"/>
-    <hyperlink ref="A205" r:id="rId206" display="powiat opoczyński"/>
-    <hyperlink ref="A206" r:id="rId207" display="Opole"/>
-    <hyperlink ref="A207" r:id="rId208" display="powiat opolski"/>
-    <hyperlink ref="A208" r:id="rId209" display="powiat opolski"/>
-    <hyperlink ref="A209" r:id="rId210" display="powiat ostrołęcki"/>
-    <hyperlink ref="A210" r:id="rId211" display="Ostrołęka"/>
-    <hyperlink ref="A211" r:id="rId212" display="powiat ostrowiecki"/>
-    <hyperlink ref="A212" r:id="rId213" display="powiat ostrowski"/>
-    <hyperlink ref="A213" r:id="rId214" display="powiat ostrowski"/>
-    <hyperlink ref="A214" r:id="rId215" display="powiat ostródzki"/>
-    <hyperlink ref="A215" r:id="rId216" display="powiat ostrzeszowski"/>
-    <hyperlink ref="A216" r:id="rId217" display="powiat oświęcimski"/>
-    <hyperlink ref="A217" r:id="rId218" display="powiat otwocki"/>
-    <hyperlink ref="A218" r:id="rId219" display="powiat pabianicki"/>
-    <hyperlink ref="A219" r:id="rId220" display="powiat pajęczański"/>
-    <hyperlink ref="A220" r:id="rId221" display="powiat parczewski"/>
-    <hyperlink ref="A221" r:id="rId222" display="powiat piaseczyński"/>
-    <hyperlink ref="A222" r:id="rId223" display="Piekary Śląskie"/>
-    <hyperlink ref="A223" r:id="rId224" display="powiat pilski"/>
-    <hyperlink ref="A224" r:id="rId225" display="powiat pińczowski"/>
-    <hyperlink ref="A225" r:id="rId226" display="powiat piotrkowski"/>
-    <hyperlink ref="A226" r:id="rId227" display="Piotrków Trybunalski"/>
-    <hyperlink ref="A227" r:id="rId228" display="powiat piski"/>
-    <hyperlink ref="A228" r:id="rId229" display="powiat pleszewski"/>
-    <hyperlink ref="A229" r:id="rId230" display="Płock"/>
-    <hyperlink ref="A230" r:id="rId231" display="powiat płocki"/>
-    <hyperlink ref="A231" r:id="rId232" display="powiat płoński"/>
-    <hyperlink ref="A232" r:id="rId233" display="powiat poddębicki"/>
-    <hyperlink ref="A233" r:id="rId234" display="powiat policki"/>
-    <hyperlink ref="A234" r:id="rId235" display="powiat polkowicki"/>
-    <hyperlink ref="A235" r:id="rId236" display="Poznań"/>
-    <hyperlink ref="A236" r:id="rId237" display="powiat poznański"/>
-    <hyperlink ref="A237" r:id="rId238" display="powiat proszowicki"/>
-    <hyperlink ref="A238" r:id="rId239" display="powiat prudnicki"/>
-    <hyperlink ref="A239" r:id="rId240" display="powiat pruszkowski"/>
-    <hyperlink ref="A240" r:id="rId241" display="powiat przasnyski"/>
-    <hyperlink ref="A241" r:id="rId242" display="powiat przemyski"/>
-    <hyperlink ref="A242" r:id="rId243" display="Przemyśl"/>
-    <hyperlink ref="A243" r:id="rId244" display="powiat przeworski"/>
-    <hyperlink ref="A244" r:id="rId245" display="powiat przysuski"/>
-    <hyperlink ref="A245" r:id="rId246" display="powiat pszczyński"/>
-    <hyperlink ref="A246" r:id="rId247" display="powiat pucki"/>
-    <hyperlink ref="A247" r:id="rId248" display="powiat puławski"/>
-    <hyperlink ref="A248" r:id="rId249" display="powiat pułtuski"/>
-    <hyperlink ref="A249" r:id="rId250" display="powiat pyrzycki"/>
-    <hyperlink ref="A250" r:id="rId251" display="powiat raciborski"/>
-    <hyperlink ref="A251" r:id="rId252" display="Radom"/>
-    <hyperlink ref="A252" r:id="rId253" display="powiat radomski"/>
-    <hyperlink ref="A253" r:id="rId254" display="powiat radomszczański"/>
-    <hyperlink ref="A254" r:id="rId255" display="powiat radziejowski"/>
-    <hyperlink ref="A255" r:id="rId256" display="powiat radzyński"/>
-    <hyperlink ref="A256" r:id="rId257" display="powiat rawicki"/>
-    <hyperlink ref="A257" r:id="rId258" display="powiat rawski"/>
-    <hyperlink ref="A258" r:id="rId259" display="powiat ropczycko-sędziszowski"/>
-    <hyperlink ref="A259" r:id="rId260" display="Ruda Śląska"/>
-    <hyperlink ref="A260" r:id="rId261" display="powiat rybnicki"/>
-    <hyperlink ref="A261" r:id="rId262" display="Rybnik"/>
-    <hyperlink ref="A262" r:id="rId263" display="powiat rycki"/>
-    <hyperlink ref="A263" r:id="rId264" display="powiat rypiński"/>
-    <hyperlink ref="A264" r:id="rId265" display="powiat rzeszowski"/>
-    <hyperlink ref="A265" r:id="rId266" display="Rzeszów"/>
-    <hyperlink ref="A266" r:id="rId267" display="powiat sandomierski"/>
-    <hyperlink ref="A267" r:id="rId268" display="powiat sanocki"/>
-    <hyperlink ref="A268" r:id="rId269" display="powiat sejneński"/>
-    <hyperlink ref="A269" r:id="rId270" display="powiat sępoleński"/>
-    <hyperlink ref="A270" r:id="rId271" display="Siedlce"/>
-    <hyperlink ref="A271" r:id="rId272" display="powiat siedlecki"/>
-    <hyperlink ref="A272" r:id="rId273" display="Siemianowice Śląskie"/>
-    <hyperlink ref="A273" r:id="rId274" display="powiat siemiatycki"/>
-    <hyperlink ref="A274" r:id="rId275" display="powiat sieradzki"/>
-    <hyperlink ref="A275" r:id="rId276" display="powiat sierpecki"/>
-    <hyperlink ref="A276" r:id="rId277" display="powiat skarżyski"/>
-    <hyperlink ref="A277" r:id="rId278" display="Skierniewice"/>
-    <hyperlink ref="A278" r:id="rId279" display="powiat skierniewicki"/>
-    <hyperlink ref="A279" r:id="rId280" display="powiat sławieński"/>
-    <hyperlink ref="A280" r:id="rId281" display="powiat słubicki"/>
-    <hyperlink ref="A281" r:id="rId282" display="powiat słupecki"/>
-    <hyperlink ref="A282" r:id="rId283" display="Słupsk"/>
-    <hyperlink ref="A283" r:id="rId284" display="powiat słupski"/>
-    <hyperlink ref="A284" r:id="rId285" display="powiat sochaczewski"/>
-    <hyperlink ref="A285" r:id="rId286" display="powiat sokołowski"/>
-    <hyperlink ref="A286" r:id="rId287" display="powiat sokólski"/>
-    <hyperlink ref="A287" r:id="rId288" display="Sopot"/>
-    <hyperlink ref="A288" r:id="rId289" display="Sosnowiec"/>
-    <hyperlink ref="A289" r:id="rId290" display="powiat stalowowolski"/>
-    <hyperlink ref="A290" r:id="rId291" display="powiat starachowicki"/>
-    <hyperlink ref="A291" r:id="rId292" display="powiat stargardzki"/>
-    <hyperlink ref="A292" r:id="rId293" display="powiat starogardzki"/>
-    <hyperlink ref="A293" r:id="rId294" display="powiat staszowski"/>
-    <hyperlink ref="A294" r:id="rId295" display="powiat strzelecki"/>
-    <hyperlink ref="A295" r:id="rId296" display="powiat strzelecko-drezdenecki"/>
-    <hyperlink ref="A296" r:id="rId297" display="powiat strzeliński"/>
-    <hyperlink ref="A297" r:id="rId298" display="powiat strzyżowski"/>
-    <hyperlink ref="A298" r:id="rId299" display="powiat sulęciński"/>
-    <hyperlink ref="A299" r:id="rId300" display="powiat suski"/>
-    <hyperlink ref="A300" r:id="rId301" display="powiat suwalski"/>
-    <hyperlink ref="A301" r:id="rId302" display="Suwałki"/>
-    <hyperlink ref="A302" r:id="rId303" display="powiat szamotulski"/>
-    <hyperlink ref="A303" r:id="rId304" display="Szczecin"/>
-    <hyperlink ref="A304" r:id="rId305" display="powiat szczecinecki"/>
-    <hyperlink ref="A305" r:id="rId306" display="powiat szczycieński"/>
-    <hyperlink ref="A306" r:id="rId307" display="powiat sztumski"/>
-    <hyperlink ref="A307" r:id="rId308" display="powiat szydłowiecki"/>
-    <hyperlink ref="A308" r:id="rId309" display="powiat średzki"/>
-    <hyperlink ref="A309" r:id="rId310" display="powiat średzki"/>
-    <hyperlink ref="A310" r:id="rId311" display="powiat śremski"/>
-    <hyperlink ref="A311" r:id="rId312" display="powiat świdnicki"/>
-    <hyperlink ref="A312" r:id="rId313" display="powiat świdnicki"/>
-    <hyperlink ref="A313" r:id="rId314" display="powiat świdwiński"/>
-    <hyperlink ref="A314" r:id="rId315" display="powiat świebodziński"/>
-    <hyperlink ref="A315" r:id="rId316" display="powiat świecki"/>
-    <hyperlink ref="A316" r:id="rId317" display="Świętochłowice"/>
-    <hyperlink ref="A317" r:id="rId318" display="Świnoujście"/>
-    <hyperlink ref="A318" r:id="rId319" display="Tarnobrzeg"/>
-    <hyperlink ref="A319" r:id="rId320" display="powiat tarnobrzeski"/>
-    <hyperlink ref="A320" r:id="rId321" display="powiat tarnogórski"/>
-    <hyperlink ref="A321" r:id="rId322" display="powiat tarnowski"/>
-    <hyperlink ref="A322" r:id="rId323" display="Tarnów"/>
-    <hyperlink ref="A323" r:id="rId324" display="powiat tatrzański"/>
-    <hyperlink ref="A324" r:id="rId325" display="powiat tczewski"/>
-    <hyperlink ref="A325" r:id="rId326" display="powiat tomaszowski"/>
-    <hyperlink ref="A326" r:id="rId327" display="powiat tomaszowski"/>
-    <hyperlink ref="A327" r:id="rId328" display="Toruń"/>
-    <hyperlink ref="A328" r:id="rId329" display="powiat toruński"/>
-    <hyperlink ref="A329" r:id="rId330" display="powiat trzebnicki"/>
-    <hyperlink ref="A330" r:id="rId331" display="powiat tucholski"/>
-    <hyperlink ref="A331" r:id="rId332" display="powiat turecki"/>
-    <hyperlink ref="A332" r:id="rId333" display="Tychy"/>
-    <hyperlink ref="A333" r:id="rId334" display="powiat wadowicki"/>
-    <hyperlink ref="A334" r:id="rId335" display="Wałbrzych"/>
-    <hyperlink ref="A335" r:id="rId336" display="powiat wałbrzyski"/>
-    <hyperlink ref="A336" r:id="rId337" display="powiat wałecki"/>
-    <hyperlink ref="A337" r:id="rId338" display="Warszawa"/>
-    <hyperlink ref="A338" r:id="rId339" display="powiat warszawski zachodni"/>
-    <hyperlink ref="A339" r:id="rId340" display="powiat wąbrzeski"/>
-    <hyperlink ref="A340" r:id="rId341" display="powiat wągrowiecki"/>
-    <hyperlink ref="A341" r:id="rId342" display="powiat wejherowski"/>
-    <hyperlink ref="A342" r:id="rId343" display="powiat węgorzewski"/>
-    <hyperlink ref="A343" r:id="rId344" display="powiat węgrowski"/>
-    <hyperlink ref="A344" r:id="rId345" display="powiat wielicki"/>
-    <hyperlink ref="A345" r:id="rId346" display="powiat wieluński"/>
-    <hyperlink ref="A346" r:id="rId347" display="powiat wieruszowski"/>
-    <hyperlink ref="A347" r:id="rId348" display="Włocławek"/>
-    <hyperlink ref="A348" r:id="rId349" display="powiat włocławski"/>
-    <hyperlink ref="A349" r:id="rId350" display="powiat włodawski"/>
-    <hyperlink ref="A350" r:id="rId351" display="powiat włoszczowski"/>
-    <hyperlink ref="A351" r:id="rId352" display="powiat wodzisławski"/>
-    <hyperlink ref="A352" r:id="rId353" display="powiat wolsztyński"/>
-    <hyperlink ref="A353" r:id="rId354" display="powiat wołomiński"/>
-    <hyperlink ref="A354" r:id="rId355" display="powiat wołowski"/>
-    <hyperlink ref="A355" r:id="rId356" display="Wrocław"/>
-    <hyperlink ref="A356" r:id="rId357" display="powiat wrocławski"/>
-    <hyperlink ref="A357" r:id="rId358" display="powiat wrzesiński"/>
-    <hyperlink ref="A358" r:id="rId359" display="powiat wschowski"/>
-    <hyperlink ref="A359" r:id="rId360" display="powiat wysokomazowiecki"/>
-    <hyperlink ref="A360" r:id="rId361" display="powiat wyszkowski"/>
-    <hyperlink ref="A361" r:id="rId362" display="Zabrze"/>
-    <hyperlink ref="A362" r:id="rId363" display="powiat zambrowski"/>
-    <hyperlink ref="A363" r:id="rId364" display="powiat zamojski"/>
-    <hyperlink ref="A364" r:id="rId365" display="Zamość"/>
-    <hyperlink ref="A365" r:id="rId366" display="powiat zawierciański"/>
-    <hyperlink ref="A366" r:id="rId367" display="powiat ząbkowicki"/>
-    <hyperlink ref="A367" r:id="rId368" display="powiat zduńskowolski"/>
-    <hyperlink ref="A368" r:id="rId369" display="powiat zgierski"/>
-    <hyperlink ref="A369" r:id="rId370" display="powiat zgorzelecki"/>
-    <hyperlink ref="A370" r:id="rId371" display="Zielona Góra"/>
-    <hyperlink ref="A371" r:id="rId372" display="powiat zielonogórski"/>
-    <hyperlink ref="A372" r:id="rId373" display="powiat złotoryjski"/>
-    <hyperlink ref="A373" r:id="rId374" display="powiat złotowski"/>
-    <hyperlink ref="A374" r:id="rId375" display="powiat zwoleński"/>
-    <hyperlink ref="A375" r:id="rId376" display="powiat żagański"/>
-    <hyperlink ref="A376" r:id="rId377" display="powiat żarski"/>
-    <hyperlink ref="A377" r:id="rId378" display="powiat żniński"/>
-    <hyperlink ref="A378" r:id="rId379" display="Żory"/>
-    <hyperlink ref="A379" r:id="rId380" display="powiat żuromiński"/>
-    <hyperlink ref="A380" r:id="rId381" display="powiat żyrardowski"/>
-    <hyperlink ref="A381" r:id="rId382" display="powiat żywiecki"/>
+    <hyperlink ref="A30" r:id="rId30" display="Bytom"/>
+    <hyperlink ref="A31" r:id="rId31" display="powiat bytowski"/>
+    <hyperlink ref="A33" r:id="rId32" display="powiat chełmiński"/>
+    <hyperlink ref="A34" r:id="rId33" display="powiat chełmski"/>
+    <hyperlink ref="A35" r:id="rId34" display="powiat chodzieski"/>
+    <hyperlink ref="A36" r:id="rId35" display="powiat chojnicki"/>
+    <hyperlink ref="A37" r:id="rId36" display="Chorzów"/>
+    <hyperlink ref="A38" r:id="rId37" display="powiat choszczeński"/>
+    <hyperlink ref="A39" r:id="rId38" display="powiat chrzanowski"/>
+    <hyperlink ref="A40" r:id="rId39" display="powiat ciechanowski"/>
+    <hyperlink ref="A41" r:id="rId40" display="powiat cieszyński"/>
+    <hyperlink ref="A42" r:id="rId41" display="powiat czarnkowsko-trzcianecki"/>
+    <hyperlink ref="A43" r:id="rId42" display="Częstochowa"/>
+    <hyperlink ref="A44" r:id="rId43" display="powiat częstochowski"/>
+    <hyperlink ref="A45" r:id="rId44" display="powiat człuchowski"/>
+    <hyperlink ref="A46" r:id="rId45" display="Dąbrowa Górnicza"/>
+    <hyperlink ref="A47" r:id="rId46" display="powiat dąbrowski"/>
+    <hyperlink ref="A48" r:id="rId47" display="powiat dębicki"/>
+    <hyperlink ref="A49" r:id="rId48" display="powiat drawski"/>
+    <hyperlink ref="A50" r:id="rId49" display="powiat działdowski"/>
+    <hyperlink ref="A51" r:id="rId50" display="powiat dzierżoniowski"/>
+    <hyperlink ref="A52" r:id="rId51" display="Elbląg"/>
+    <hyperlink ref="A53" r:id="rId52" display="powiat elbląski"/>
+    <hyperlink ref="A54" r:id="rId53" display="powiat ełcki"/>
+    <hyperlink ref="A55" r:id="rId54" display="powiat garwoliński"/>
+    <hyperlink ref="A56" r:id="rId55" display="Gdańsk"/>
+    <hyperlink ref="A57" r:id="rId56" display="powiat gdański"/>
+    <hyperlink ref="A58" r:id="rId57" display="Gdynia"/>
+    <hyperlink ref="A59" r:id="rId58" display="powiat giżycki"/>
+    <hyperlink ref="A60" r:id="rId59" display="Gliwice"/>
+    <hyperlink ref="A61" r:id="rId60" display="powiat gliwicki"/>
+    <hyperlink ref="A62" r:id="rId61" display="powiat głogowski"/>
+    <hyperlink ref="A63" r:id="rId62" display="powiat głubczycki"/>
+    <hyperlink ref="A64" r:id="rId63" display="powiat gnieźnieński"/>
+    <hyperlink ref="A65" r:id="rId64" display="powiat goleniowski"/>
+    <hyperlink ref="A66" r:id="rId65" display="powiat golubsko-dobrzyński"/>
+    <hyperlink ref="A67" r:id="rId66" display="powiat gołdapski"/>
+    <hyperlink ref="A68" r:id="rId67" display="powiat gorlicki"/>
+    <hyperlink ref="A69" r:id="rId68" display="powiat gorzowski"/>
+    <hyperlink ref="A70" r:id="rId69" display="Gorzów Wielkopolski"/>
+    <hyperlink ref="A71" r:id="rId70" display="powiat gostyniński"/>
+    <hyperlink ref="A72" r:id="rId71" display="powiat gostyński"/>
+    <hyperlink ref="A73" r:id="rId72" display="powiat górowski"/>
+    <hyperlink ref="A74" r:id="rId73" display="powiat grajewski"/>
+    <hyperlink ref="A75" r:id="rId74" display="powiat grodziski"/>
+    <hyperlink ref="A76" r:id="rId75" display="powiat grodziski"/>
+    <hyperlink ref="A77" r:id="rId76" display="powiat grójecki"/>
+    <hyperlink ref="A78" r:id="rId77" display="Grudziądz"/>
+    <hyperlink ref="A79" r:id="rId78" display="powiat grudziądzki"/>
+    <hyperlink ref="A80" r:id="rId79" display="powiat gryficki"/>
+    <hyperlink ref="A81" r:id="rId80" display="powiat gryfiński"/>
+    <hyperlink ref="A82" r:id="rId81" display="powiat hajnowski"/>
+    <hyperlink ref="A83" r:id="rId82" display="powiat hrubieszowski"/>
+    <hyperlink ref="A84" r:id="rId83" display="powiat iławski"/>
+    <hyperlink ref="A85" r:id="rId84" display="powiat inowrocławski"/>
+    <hyperlink ref="A86" r:id="rId85" display="powiat janowski"/>
+    <hyperlink ref="A87" r:id="rId86" display="powiat jarociński"/>
+    <hyperlink ref="A88" r:id="rId87" display="powiat jarosławski"/>
+    <hyperlink ref="A89" r:id="rId88" display="powiat jasielski"/>
+    <hyperlink ref="A90" r:id="rId89" display="Jastrzębie-Zdrój"/>
+    <hyperlink ref="A91" r:id="rId90" display="powiat jaworski"/>
+    <hyperlink ref="A92" r:id="rId91" display="Jaworzno"/>
+    <hyperlink ref="A93" r:id="rId92" display="Jelenia Góra"/>
+    <hyperlink ref="A94" r:id="rId93" display="powiat jeleniogórski"/>
+    <hyperlink ref="A95" r:id="rId94" display="powiat jędrzejowski"/>
+    <hyperlink ref="A96" r:id="rId95" display="powiat kaliski"/>
+    <hyperlink ref="A97" r:id="rId96" display="Kalisz"/>
+    <hyperlink ref="A98" r:id="rId97" display="powiat kamiennogórski"/>
+    <hyperlink ref="A99" r:id="rId98" display="powiat kamieński"/>
+    <hyperlink ref="A100" r:id="rId99" display="powiat kartuski"/>
+    <hyperlink ref="A101" r:id="rId100" display="Katowice"/>
+    <hyperlink ref="A102" r:id="rId101" display="powiat kazimierski"/>
+    <hyperlink ref="A103" r:id="rId102" display="powiat kędzierzyńsko-kozielski"/>
+    <hyperlink ref="A104" r:id="rId103" display="powiat kępiński"/>
+    <hyperlink ref="A105" r:id="rId104" display="powiat kętrzyński"/>
+    <hyperlink ref="A106" r:id="rId105" display="Kielce"/>
+    <hyperlink ref="A107" r:id="rId106" display="powiat kielecki"/>
+    <hyperlink ref="A108" r:id="rId107" display="powiat kluczborski"/>
+    <hyperlink ref="A109" r:id="rId108" display="powiat kłobucki"/>
+    <hyperlink ref="A110" r:id="rId109" display="powiat kłodzki"/>
+    <hyperlink ref="A111" r:id="rId110" display="powiat kolbuszowski"/>
+    <hyperlink ref="A112" r:id="rId111" display="powiat kolneński"/>
+    <hyperlink ref="A113" r:id="rId112" display="powiat kolski"/>
+    <hyperlink ref="A114" r:id="rId113" display="powiat kołobrzeski"/>
+    <hyperlink ref="A115" r:id="rId114" display="powiat konecki"/>
+    <hyperlink ref="A116" r:id="rId115" display="Konin"/>
+    <hyperlink ref="A117" r:id="rId116" display="powiat koniński"/>
+    <hyperlink ref="A118" r:id="rId117" display="Koszalin"/>
+    <hyperlink ref="A119" r:id="rId118" display="powiat koszaliński"/>
+    <hyperlink ref="A120" r:id="rId119" display="powiat kościański"/>
+    <hyperlink ref="A121" r:id="rId120" display="powiat kościerski"/>
+    <hyperlink ref="A122" r:id="rId121" display="powiat kozienicki"/>
+    <hyperlink ref="A123" r:id="rId122" display="powiat krakowski"/>
+    <hyperlink ref="A124" r:id="rId123" display="Kraków"/>
+    <hyperlink ref="A125" r:id="rId124" display="powiat krapkowicki"/>
+    <hyperlink ref="A126" r:id="rId125" display="powiat krasnostawski"/>
+    <hyperlink ref="A127" r:id="rId126" display="powiat kraśnicki"/>
+    <hyperlink ref="A128" r:id="rId127" display="Krosno"/>
+    <hyperlink ref="A129" r:id="rId128" display="powiat krośnieński"/>
+    <hyperlink ref="A130" r:id="rId129" display="powiat krośnieński"/>
+    <hyperlink ref="A131" r:id="rId130" display="powiat krotoszyński"/>
+    <hyperlink ref="A132" r:id="rId131" display="powiat kutnowski"/>
+    <hyperlink ref="A133" r:id="rId132" display="powiat kwidzyński"/>
+    <hyperlink ref="A134" r:id="rId133" display="powiat legionowski"/>
+    <hyperlink ref="A135" r:id="rId134" display="Legnica"/>
+    <hyperlink ref="A136" r:id="rId135" display="powiat legnicki"/>
+    <hyperlink ref="A137" r:id="rId136" display="powiat leski"/>
+    <hyperlink ref="A138" r:id="rId137" display="powiat leszczyński"/>
+    <hyperlink ref="A139" r:id="rId138" display="Leszno"/>
+    <hyperlink ref="A140" r:id="rId139" display="powiat leżajski"/>
+    <hyperlink ref="A141" r:id="rId140" display="powiat lęborski"/>
+    <hyperlink ref="A142" r:id="rId141" display="powiat lidzbarski"/>
+    <hyperlink ref="A143" r:id="rId142" display="powiat limanowski"/>
+    <hyperlink ref="A144" r:id="rId143" display="powiat lipnowski"/>
+    <hyperlink ref="A145" r:id="rId144" display="powiat lipski"/>
+    <hyperlink ref="A146" r:id="rId145" display="powiat lubaczowski"/>
+    <hyperlink ref="A147" r:id="rId146" display="powiat lubański"/>
+    <hyperlink ref="A148" r:id="rId147" display="powiat lubartowski"/>
+    <hyperlink ref="A149" r:id="rId148" display="powiat lubelski"/>
+    <hyperlink ref="A150" r:id="rId149" display="powiat lubiński"/>
+    <hyperlink ref="A151" r:id="rId150" display="Lublin"/>
+    <hyperlink ref="A152" r:id="rId151" display="powiat lubliniecki"/>
+    <hyperlink ref="A153" r:id="rId152" display="powiat lwówecki"/>
+    <hyperlink ref="A154" r:id="rId153" display="powiat łańcucki"/>
+    <hyperlink ref="A155" r:id="rId154" display="powiat łaski"/>
+    <hyperlink ref="A156" r:id="rId155" display="powiat łęczycki"/>
+    <hyperlink ref="A157" r:id="rId156" display="powiat łęczyński"/>
+    <hyperlink ref="A158" r:id="rId157" display="powiat łobeski"/>
+    <hyperlink ref="A159" r:id="rId158" display="Łomża"/>
+    <hyperlink ref="A160" r:id="rId159" display="powiat łomżyński"/>
+    <hyperlink ref="A161" r:id="rId160" display="powiat łosicki"/>
+    <hyperlink ref="A162" r:id="rId161" display="powiat łowicki"/>
+    <hyperlink ref="A163" r:id="rId162" display="powiat łódzki wschodni"/>
+    <hyperlink ref="A164" r:id="rId163" display="Łódź"/>
+    <hyperlink ref="A165" r:id="rId164" display="powiat łukowski"/>
+    <hyperlink ref="A166" r:id="rId165" display="powiat makowski"/>
+    <hyperlink ref="A167" r:id="rId166" display="powiat malborski"/>
+    <hyperlink ref="A168" r:id="rId167" display="powiat miechowski"/>
+    <hyperlink ref="A169" r:id="rId168" display="powiat mielecki"/>
+    <hyperlink ref="A170" r:id="rId169" display="powiat międzychodzki"/>
+    <hyperlink ref="A171" r:id="rId170" display="powiat międzyrzecki"/>
+    <hyperlink ref="A172" r:id="rId171" display="powiat mikołowski"/>
+    <hyperlink ref="A173" r:id="rId172" display="powiat milicki"/>
+    <hyperlink ref="A174" r:id="rId173" display="powiat miński"/>
+    <hyperlink ref="A175" r:id="rId174" display="powiat mławski"/>
+    <hyperlink ref="A176" r:id="rId175" display="powiat mogileński"/>
+    <hyperlink ref="A177" r:id="rId176" display="powiat moniecki"/>
+    <hyperlink ref="A178" r:id="rId177" display="powiat mrągowski"/>
+    <hyperlink ref="A179" r:id="rId178" display="Mysłowice"/>
+    <hyperlink ref="A180" r:id="rId179" display="powiat myszkowski"/>
+    <hyperlink ref="A181" r:id="rId180" display="powiat myślenicki"/>
+    <hyperlink ref="A182" r:id="rId181" display="powiat myśliborski"/>
+    <hyperlink ref="A183" r:id="rId182" display="powiat nakielski"/>
+    <hyperlink ref="A184" r:id="rId183" display="powiat namysłowski"/>
+    <hyperlink ref="A185" r:id="rId184" display="powiat nidzicki"/>
+    <hyperlink ref="A186" r:id="rId185" display="powiat niżański"/>
+    <hyperlink ref="A187" r:id="rId186" display="powiat nowodworski"/>
+    <hyperlink ref="A188" r:id="rId187" display="powiat nowodworski"/>
+    <hyperlink ref="A189" r:id="rId188" display="powiat nowomiejski"/>
+    <hyperlink ref="A190" r:id="rId189" display="powiat nowosądecki"/>
+    <hyperlink ref="A191" r:id="rId190" display="powiat nowosolski"/>
+    <hyperlink ref="A192" r:id="rId191" display="powiat nowotarski"/>
+    <hyperlink ref="A193" r:id="rId192" display="powiat nowotomyski"/>
+    <hyperlink ref="A194" r:id="rId193" display="Nowy Sącz"/>
+    <hyperlink ref="A195" r:id="rId194" display="powiat nyski"/>
+    <hyperlink ref="A196" r:id="rId195" display="powiat obornicki"/>
+    <hyperlink ref="A197" r:id="rId196" display="powiat olecki"/>
+    <hyperlink ref="A198" r:id="rId197" display="powiat oleski"/>
+    <hyperlink ref="A199" r:id="rId198" display="powiat oleśnicki"/>
+    <hyperlink ref="A200" r:id="rId199" display="powiat olkuski"/>
+    <hyperlink ref="A201" r:id="rId200" display="Olsztyn"/>
+    <hyperlink ref="A202" r:id="rId201" display="powiat olsztyński"/>
+    <hyperlink ref="A203" r:id="rId202" display="powiat oławski"/>
+    <hyperlink ref="A204" r:id="rId203" display="powiat opatowski"/>
+    <hyperlink ref="A205" r:id="rId204" display="powiat opoczyński"/>
+    <hyperlink ref="A206" r:id="rId205" display="Opole"/>
+    <hyperlink ref="A207" r:id="rId206" display="powiat opolski"/>
+    <hyperlink ref="A208" r:id="rId207" display="powiat opolski"/>
+    <hyperlink ref="A209" r:id="rId208" display="powiat ostrołęcki"/>
+    <hyperlink ref="A210" r:id="rId209" display="Ostrołęka"/>
+    <hyperlink ref="A211" r:id="rId210" display="powiat ostrowiecki"/>
+    <hyperlink ref="A212" r:id="rId211" display="powiat ostrowski"/>
+    <hyperlink ref="A213" r:id="rId212" display="powiat ostrowski"/>
+    <hyperlink ref="A214" r:id="rId213" display="powiat ostródzki"/>
+    <hyperlink ref="A215" r:id="rId214" display="powiat ostrzeszowski"/>
+    <hyperlink ref="A216" r:id="rId215" display="powiat oświęcimski"/>
+    <hyperlink ref="A217" r:id="rId216" display="powiat otwocki"/>
+    <hyperlink ref="A218" r:id="rId217" display="powiat pabianicki"/>
+    <hyperlink ref="A219" r:id="rId218" display="powiat pajęczański"/>
+    <hyperlink ref="A220" r:id="rId219" display="powiat parczewski"/>
+    <hyperlink ref="A221" r:id="rId220" display="powiat piaseczyński"/>
+    <hyperlink ref="A222" r:id="rId221" display="Piekary Śląskie"/>
+    <hyperlink ref="A223" r:id="rId222" display="powiat pilski"/>
+    <hyperlink ref="A224" r:id="rId223" display="powiat pińczowski"/>
+    <hyperlink ref="A225" r:id="rId224" display="powiat piotrkowski"/>
+    <hyperlink ref="A226" r:id="rId225" display="Piotrków Trybunalski"/>
+    <hyperlink ref="A227" r:id="rId226" display="powiat piski"/>
+    <hyperlink ref="A228" r:id="rId227" display="powiat pleszewski"/>
+    <hyperlink ref="A229" r:id="rId228" display="Płock"/>
+    <hyperlink ref="A230" r:id="rId229" display="powiat płocki"/>
+    <hyperlink ref="A231" r:id="rId230" display="powiat płoński"/>
+    <hyperlink ref="A232" r:id="rId231" display="powiat poddębicki"/>
+    <hyperlink ref="A233" r:id="rId232" display="powiat policki"/>
+    <hyperlink ref="A234" r:id="rId233" display="powiat polkowicki"/>
+    <hyperlink ref="A235" r:id="rId234" display="Poznań"/>
+    <hyperlink ref="A236" r:id="rId235" display="powiat poznański"/>
+    <hyperlink ref="A237" r:id="rId236" display="powiat proszowicki"/>
+    <hyperlink ref="A238" r:id="rId237" display="powiat prudnicki"/>
+    <hyperlink ref="A239" r:id="rId238" display="powiat pruszkowski"/>
+    <hyperlink ref="A240" r:id="rId239" display="powiat przasnyski"/>
+    <hyperlink ref="A241" r:id="rId240" display="powiat przemyski"/>
+    <hyperlink ref="A242" r:id="rId241" display="Przemyśl"/>
+    <hyperlink ref="A243" r:id="rId242" display="powiat przeworski"/>
+    <hyperlink ref="A244" r:id="rId243" display="powiat przysuski"/>
+    <hyperlink ref="A245" r:id="rId244" display="powiat pszczyński"/>
+    <hyperlink ref="A246" r:id="rId245" display="powiat pucki"/>
+    <hyperlink ref="A247" r:id="rId246" display="powiat puławski"/>
+    <hyperlink ref="A248" r:id="rId247" display="powiat pułtuski"/>
+    <hyperlink ref="A249" r:id="rId248" display="powiat pyrzycki"/>
+    <hyperlink ref="A250" r:id="rId249" display="powiat raciborski"/>
+    <hyperlink ref="A251" r:id="rId250" display="Radom"/>
+    <hyperlink ref="A252" r:id="rId251" display="powiat radomski"/>
+    <hyperlink ref="A253" r:id="rId252" display="powiat radomszczański"/>
+    <hyperlink ref="A254" r:id="rId253" display="powiat radziejowski"/>
+    <hyperlink ref="A255" r:id="rId254" display="powiat radzyński"/>
+    <hyperlink ref="A256" r:id="rId255" display="powiat rawicki"/>
+    <hyperlink ref="A257" r:id="rId256" display="powiat rawski"/>
+    <hyperlink ref="A258" r:id="rId257" display="powiat ropczycko-sędziszowski"/>
+    <hyperlink ref="A259" r:id="rId258" display="Ruda Śląska"/>
+    <hyperlink ref="A260" r:id="rId259" display="powiat rybnicki"/>
+    <hyperlink ref="A261" r:id="rId260" display="Rybnik"/>
+    <hyperlink ref="A262" r:id="rId261" display="powiat rycki"/>
+    <hyperlink ref="A263" r:id="rId262" display="powiat rypiński"/>
+    <hyperlink ref="A264" r:id="rId263" display="powiat rzeszowski"/>
+    <hyperlink ref="A265" r:id="rId264" display="Rzeszów"/>
+    <hyperlink ref="A266" r:id="rId265" display="powiat sandomierski"/>
+    <hyperlink ref="A267" r:id="rId266" display="powiat sanocki"/>
+    <hyperlink ref="A268" r:id="rId267" display="powiat sejneński"/>
+    <hyperlink ref="A269" r:id="rId268" display="powiat sępoleński"/>
+    <hyperlink ref="A270" r:id="rId269" display="Siedlce"/>
+    <hyperlink ref="A271" r:id="rId270" display="powiat siedlecki"/>
+    <hyperlink ref="A272" r:id="rId271" display="Siemianowice Śląskie"/>
+    <hyperlink ref="A273" r:id="rId272" display="powiat siemiatycki"/>
+    <hyperlink ref="A274" r:id="rId273" display="powiat sieradzki"/>
+    <hyperlink ref="A275" r:id="rId274" display="powiat sierpecki"/>
+    <hyperlink ref="A276" r:id="rId275" display="powiat skarżyski"/>
+    <hyperlink ref="A277" r:id="rId276" display="Skierniewice"/>
+    <hyperlink ref="A278" r:id="rId277" display="powiat skierniewicki"/>
+    <hyperlink ref="A279" r:id="rId278" display="powiat sławieński"/>
+    <hyperlink ref="A280" r:id="rId279" display="powiat słubicki"/>
+    <hyperlink ref="A281" r:id="rId280" display="powiat słupecki"/>
+    <hyperlink ref="A282" r:id="rId281" display="Słupsk"/>
+    <hyperlink ref="A283" r:id="rId282" display="powiat słupski"/>
+    <hyperlink ref="A284" r:id="rId283" display="powiat sochaczewski"/>
+    <hyperlink ref="A285" r:id="rId284" display="powiat sokołowski"/>
+    <hyperlink ref="A286" r:id="rId285" display="powiat sokólski"/>
+    <hyperlink ref="A287" r:id="rId286" display="Sopot"/>
+    <hyperlink ref="A288" r:id="rId287" display="Sosnowiec"/>
+    <hyperlink ref="A289" r:id="rId288" display="powiat stalowowolski"/>
+    <hyperlink ref="A290" r:id="rId289" display="powiat starachowicki"/>
+    <hyperlink ref="A291" r:id="rId290" display="powiat stargardzki"/>
+    <hyperlink ref="A292" r:id="rId291" display="powiat starogardzki"/>
+    <hyperlink ref="A293" r:id="rId292" display="powiat staszowski"/>
+    <hyperlink ref="A294" r:id="rId293" display="powiat strzelecki"/>
+    <hyperlink ref="A295" r:id="rId294" display="powiat strzelecko-drezdenecki"/>
+    <hyperlink ref="A296" r:id="rId295" display="powiat strzeliński"/>
+    <hyperlink ref="A297" r:id="rId296" display="powiat strzyżowski"/>
+    <hyperlink ref="A298" r:id="rId297" display="powiat sulęciński"/>
+    <hyperlink ref="A299" r:id="rId298" display="powiat suski"/>
+    <hyperlink ref="A300" r:id="rId299" display="powiat suwalski"/>
+    <hyperlink ref="A301" r:id="rId300" display="Suwałki"/>
+    <hyperlink ref="A302" r:id="rId301" display="powiat szamotulski"/>
+    <hyperlink ref="A303" r:id="rId302" display="Szczecin"/>
+    <hyperlink ref="A304" r:id="rId303" display="powiat szczecinecki"/>
+    <hyperlink ref="A305" r:id="rId304" display="powiat szczycieński"/>
+    <hyperlink ref="A306" r:id="rId305" display="powiat sztumski"/>
+    <hyperlink ref="A307" r:id="rId306" display="powiat szydłowiecki"/>
+    <hyperlink ref="A308" r:id="rId307" display="powiat średzki"/>
+    <hyperlink ref="A309" r:id="rId308" display="powiat średzki"/>
+    <hyperlink ref="A310" r:id="rId309" display="powiat śremski"/>
+    <hyperlink ref="A311" r:id="rId310" display="powiat świdnicki"/>
+    <hyperlink ref="A312" r:id="rId311" display="powiat świdnicki"/>
+    <hyperlink ref="A313" r:id="rId312" display="powiat świdwiński"/>
+    <hyperlink ref="A314" r:id="rId313" display="powiat świebodziński"/>
+    <hyperlink ref="A315" r:id="rId314" display="powiat świecki"/>
+    <hyperlink ref="A316" r:id="rId315" display="Świętochłowice"/>
+    <hyperlink ref="A317" r:id="rId316" display="Świnoujście"/>
+    <hyperlink ref="A318" r:id="rId317" display="Tarnobrzeg"/>
+    <hyperlink ref="A319" r:id="rId318" display="powiat tarnobrzeski"/>
+    <hyperlink ref="A320" r:id="rId319" display="powiat tarnogórski"/>
+    <hyperlink ref="A321" r:id="rId320" display="powiat tarnowski"/>
+    <hyperlink ref="A322" r:id="rId321" display="Tarnów"/>
+    <hyperlink ref="A323" r:id="rId322" display="powiat tatrzański"/>
+    <hyperlink ref="A324" r:id="rId323" display="powiat tczewski"/>
+    <hyperlink ref="A325" r:id="rId324" display="powiat tomaszowski"/>
+    <hyperlink ref="A326" r:id="rId325" display="powiat tomaszowski"/>
+    <hyperlink ref="A327" r:id="rId326" display="Toruń"/>
+    <hyperlink ref="A328" r:id="rId327" display="powiat toruński"/>
+    <hyperlink ref="A329" r:id="rId328" display="powiat trzebnicki"/>
+    <hyperlink ref="A330" r:id="rId329" display="powiat tucholski"/>
+    <hyperlink ref="A331" r:id="rId330" display="powiat turecki"/>
+    <hyperlink ref="A332" r:id="rId331" display="Tychy"/>
+    <hyperlink ref="A333" r:id="rId332" display="powiat wadowicki"/>
+    <hyperlink ref="A334" r:id="rId333" display="Wałbrzych"/>
+    <hyperlink ref="A335" r:id="rId334" display="powiat wałbrzyski"/>
+    <hyperlink ref="A336" r:id="rId335" display="powiat wałecki"/>
+    <hyperlink ref="A337" r:id="rId336" display="Warszawa"/>
+    <hyperlink ref="A338" r:id="rId337" display="powiat warszawski zachodni"/>
+    <hyperlink ref="A339" r:id="rId338" display="powiat wąbrzeski"/>
+    <hyperlink ref="A340" r:id="rId339" display="powiat wągrowiecki"/>
+    <hyperlink ref="A341" r:id="rId340" display="powiat wejherowski"/>
+    <hyperlink ref="A342" r:id="rId341" display="powiat węgorzewski"/>
+    <hyperlink ref="A343" r:id="rId342" display="powiat węgrowski"/>
+    <hyperlink ref="A344" r:id="rId343" display="powiat wielicki"/>
+    <hyperlink ref="A345" r:id="rId344" display="powiat wieluński"/>
+    <hyperlink ref="A346" r:id="rId345" display="powiat wieruszowski"/>
+    <hyperlink ref="A347" r:id="rId346" display="Włocławek"/>
+    <hyperlink ref="A348" r:id="rId347" display="powiat włocławski"/>
+    <hyperlink ref="A349" r:id="rId348" display="powiat włodawski"/>
+    <hyperlink ref="A350" r:id="rId349" display="powiat włoszczowski"/>
+    <hyperlink ref="A351" r:id="rId350" display="powiat wodzisławski"/>
+    <hyperlink ref="A352" r:id="rId351" display="powiat wolsztyński"/>
+    <hyperlink ref="A353" r:id="rId352" display="powiat wołomiński"/>
+    <hyperlink ref="A354" r:id="rId353" display="powiat wołowski"/>
+    <hyperlink ref="A355" r:id="rId354" display="Wrocław"/>
+    <hyperlink ref="A356" r:id="rId355" display="powiat wrocławski"/>
+    <hyperlink ref="A357" r:id="rId356" display="powiat wrzesiński"/>
+    <hyperlink ref="A358" r:id="rId357" display="powiat wschowski"/>
+    <hyperlink ref="A359" r:id="rId358" display="powiat wysokomazowiecki"/>
+    <hyperlink ref="A360" r:id="rId359" display="powiat wyszkowski"/>
+    <hyperlink ref="A361" r:id="rId360" display="Zabrze"/>
+    <hyperlink ref="A362" r:id="rId361" display="powiat zambrowski"/>
+    <hyperlink ref="A363" r:id="rId362" display="powiat zamojski"/>
+    <hyperlink ref="A364" r:id="rId363" display="Zamość"/>
+    <hyperlink ref="A365" r:id="rId364" display="powiat zawierciański"/>
+    <hyperlink ref="A366" r:id="rId365" display="powiat ząbkowicki"/>
+    <hyperlink ref="A367" r:id="rId366" display="powiat zduńskowolski"/>
+    <hyperlink ref="A368" r:id="rId367" display="powiat zgierski"/>
+    <hyperlink ref="A369" r:id="rId368" display="powiat zgorzelecki"/>
+    <hyperlink ref="A370" r:id="rId369" display="Zielona Góra"/>
+    <hyperlink ref="A371" r:id="rId370" display="powiat zielonogórski"/>
+    <hyperlink ref="A372" r:id="rId371" display="powiat złotoryjski"/>
+    <hyperlink ref="A373" r:id="rId372" display="powiat złotowski"/>
+    <hyperlink ref="A374" r:id="rId373" display="powiat zwoleński"/>
+    <hyperlink ref="A375" r:id="rId374" display="powiat żagański"/>
+    <hyperlink ref="A376" r:id="rId375" display="powiat żarski"/>
+    <hyperlink ref="A377" r:id="rId376" display="powiat żniński"/>
+    <hyperlink ref="A378" r:id="rId377" display="Żory"/>
+    <hyperlink ref="A379" r:id="rId378" display="powiat żuromiński"/>
+    <hyperlink ref="A380" r:id="rId379" display="powiat żyrardowski"/>
+    <hyperlink ref="A381" r:id="rId380" display="powiat żywiecki"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>